<commit_message>
Issue #9 Got test for JDBC connectivity working
</commit_message>
<xml_diff>
--- a/Risk Assessment/Risk Assessment ERD.xlsx
+++ b/Risk Assessment/Risk Assessment ERD.xlsx
@@ -106,6 +106,12 @@
     <t xml:space="preserve">Losing the database</t>
   </si>
   <si>
+    <t xml:space="preserve">PROBABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Will periodically back up the database on Gdrive and Git.</t>
   </si>
   <si>
@@ -119,12 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">Security flaws with sensitive information (usernames and passwords)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROBABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIGH</t>
   </si>
   <si>
     <t xml:space="preserve">Unlikely to happen during development as the application will be hosted locally. However, after development has finished, this could be considered by the security team.</t>
@@ -682,7 +682,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -699,7 +699,7 @@
   <dxfs count="120">
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -709,7 +709,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -719,7 +719,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -730,7 +730,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -740,7 +740,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -750,7 +750,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -760,7 +760,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -771,7 +771,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -781,7 +781,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -791,7 +791,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -801,7 +801,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -811,7 +811,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -821,7 +821,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -831,7 +831,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -843,7 +843,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -855,7 +855,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -867,7 +867,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -879,7 +879,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -891,7 +891,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -903,7 +903,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -915,7 +915,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -927,7 +927,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -961,7 +961,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -971,7 +971,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -981,7 +981,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -992,7 +992,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1002,7 +1002,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1012,7 +1012,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1022,7 +1022,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1033,7 +1033,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1043,7 +1043,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1053,7 +1053,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1063,7 +1063,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1073,7 +1073,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1083,7 +1083,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1093,7 +1093,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1105,7 +1105,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1117,7 +1117,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1129,7 +1129,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1141,7 +1141,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1153,7 +1153,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1165,7 +1165,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1177,7 +1177,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1189,7 +1189,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1223,7 +1223,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1233,7 +1233,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1243,7 +1243,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1254,7 +1254,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1264,7 +1264,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1274,7 +1274,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1284,7 +1284,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1295,7 +1295,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1305,7 +1305,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1315,7 +1315,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1325,7 +1325,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1335,7 +1335,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1345,7 +1345,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1355,7 +1355,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1367,7 +1367,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1379,7 +1379,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1391,7 +1391,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1403,7 +1403,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1415,7 +1415,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1427,7 +1427,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1439,7 +1439,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1451,7 +1451,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1485,7 +1485,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1495,7 +1495,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1505,7 +1505,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1516,7 +1516,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1526,7 +1526,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1536,7 +1536,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1546,7 +1546,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1557,7 +1557,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1567,7 +1567,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1577,7 +1577,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1587,7 +1587,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1597,7 +1597,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1607,7 +1607,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1617,7 +1617,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1629,7 +1629,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1641,7 +1641,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1653,7 +1653,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1665,7 +1665,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1677,7 +1677,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1689,7 +1689,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1701,7 +1701,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1713,7 +1713,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1747,7 +1747,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1757,7 +1757,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1767,7 +1767,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1778,7 +1778,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1788,7 +1788,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1798,7 +1798,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1808,7 +1808,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1819,7 +1819,7 @@
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1829,7 +1829,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1839,7 +1839,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1849,7 +1849,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1859,7 +1859,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1869,7 +1869,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1879,7 +1879,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1891,7 +1891,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1903,7 +1903,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1915,7 +1915,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1927,7 +1927,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1939,7 +1939,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1951,7 +1951,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1963,7 +1963,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -1975,7 +1975,7 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
@@ -2076,7 +2076,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>50760</xdr:colOff>
+      <xdr:colOff>51120</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>390240</xdr:rowOff>
     </xdr:from>
@@ -2084,7 +2084,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>100800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>232560</xdr:rowOff>
+      <xdr:rowOff>374400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2097,8 +2097,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17030520" y="1024560"/>
-          <a:ext cx="7097400" cy="8624160"/>
+          <a:off x="17029440" y="1024560"/>
+          <a:ext cx="7097040" cy="8623800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2113,7 +2113,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -2121,7 +2121,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>3240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2136,8 +2136,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13451760" y="0"/>
-          <a:ext cx="3531240" cy="723600"/>
+          <a:off x="13450680" y="0"/>
+          <a:ext cx="3530880" cy="723240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2163,16 +2163,16 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="41.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="41.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="1" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="1.77"/>
@@ -2186,7 +2186,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="1.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="3.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="1" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="1" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2389,16 +2389,16 @@
         <v>17</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>22</v>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="L6" s="0"/>
       <c r="P6" s="27" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R6" s="28" t="s">
         <v>18</v>
@@ -2420,24 +2420,24 @@
         <v>19</v>
       </c>
       <c r="V6" s="29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="17" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>33</v>
@@ -2459,10 +2459,10 @@
         <v>17</v>
       </c>
       <c r="R7" s="32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="T7" s="30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="L8" s="0"/>
       <c r="P8" s="34" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T8" s="33" t="s">
         <v>36</v>
@@ -2512,10 +2512,10 @@
         <v>37</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>36</v>
@@ -2524,7 +2524,7 @@
         <v>38</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>22</v>

</xml_diff>